<commit_message>
adicion de excel de componentes algunas librerias de reguladores en eagle adicion de multiplicador de cap, mod de codigo
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{D1B6F836-E699-493B-8537-3C7925BFB40A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6EFC7C08-4CF9-4D5B-9D30-520CDCDDA85E}"/>
+  <xr:revisionPtr revIDLastSave="585" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{418BC232-AD1E-47F5-B599-B1E242310D00}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
+    <workbookView xWindow="28680" yWindow="1830" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="COMPONENTES" sheetId="1" r:id="rId1"/>
+    <sheet name="CARACTERISTICAS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$A$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPONENTES!$A$3:$B$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="233">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -174,9 +175,6 @@
     <t>CRISTAL</t>
   </si>
   <si>
-    <t>OBSERVACIONES</t>
-  </si>
-  <si>
     <t>XTAL</t>
   </si>
   <si>
@@ -385,6 +383,360 @@
   </si>
   <si>
     <t>MODULO XBEE</t>
+  </si>
+  <si>
+    <t>PENDIENTES</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>0-1206-16V</t>
+  </si>
+  <si>
+    <t>0,1UF</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>0-1206-50V</t>
+  </si>
+  <si>
+    <t>1NF</t>
+  </si>
+  <si>
+    <t>0,1NF</t>
+  </si>
+  <si>
+    <t>CAPACITOR CERAMICO SMD</t>
+  </si>
+  <si>
+    <t>0-0805-10V</t>
+  </si>
+  <si>
+    <t>620PF</t>
+  </si>
+  <si>
+    <t>0-1206-10V</t>
+  </si>
+  <si>
+    <t>10UF</t>
+  </si>
+  <si>
+    <t>CAPACITOR TANTALIO SMD</t>
+  </si>
+  <si>
+    <t>CAPACITOR 4,7UF</t>
+  </si>
+  <si>
+    <t>75K</t>
+  </si>
+  <si>
+    <t>0-1206 1/4 1%</t>
+  </si>
+  <si>
+    <t>RESISTENCIA SMD</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>0-0805 1/8 1%</t>
+  </si>
+  <si>
+    <t>1,43M</t>
+  </si>
+  <si>
+    <t>MCP33121-05-E/MS</t>
+  </si>
+  <si>
+    <t>ADC 14 BIT SAR 10MSOP</t>
+  </si>
+  <si>
+    <t>OPA320</t>
+  </si>
+  <si>
+    <t>AMPLIFICADOR OPERACIONAL SOT23-5</t>
+  </si>
+  <si>
+    <t>ACS723</t>
+  </si>
+  <si>
+    <t>SENSOR DE CORRIENTE SALIDA VOLTAJE</t>
+  </si>
+  <si>
+    <t>MMCP15501-18 E/SN</t>
+  </si>
+  <si>
+    <t>1,8V</t>
+  </si>
+  <si>
+    <t>LDO 1,8 SOIC 0,1%</t>
+  </si>
+  <si>
+    <t>REF3450IDBVR</t>
+  </si>
+  <si>
+    <t>5,0V</t>
+  </si>
+  <si>
+    <t>LDO 5,0 SOT23-6</t>
+  </si>
+  <si>
+    <t>LM318</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>NE555</t>
+  </si>
+  <si>
+    <t>MULTIVIBRADOR NE555</t>
+  </si>
+  <si>
+    <t>CD4532BM</t>
+  </si>
+  <si>
+    <t>ENCODER 8 BITS MOSFET</t>
+  </si>
+  <si>
+    <t>2N2222 smd multiplicador</t>
+  </si>
+  <si>
+    <t>INA128</t>
+  </si>
+  <si>
+    <t>AMPLIFICADOR INSTRUMENTACION</t>
+  </si>
+  <si>
+    <t>LP38690DT-5</t>
+  </si>
+  <si>
+    <t>COMPONENTE</t>
+  </si>
+  <si>
+    <t>DHT22</t>
+  </si>
+  <si>
+    <t>MCP33121</t>
+  </si>
+  <si>
+    <t>R-BATH</t>
+  </si>
+  <si>
+    <t>T-BATL</t>
+  </si>
+  <si>
+    <t>XBEE</t>
+  </si>
+  <si>
+    <t>MCP6001</t>
+  </si>
+  <si>
+    <t>REF3450</t>
+  </si>
+  <si>
+    <t>LP3869</t>
+  </si>
+  <si>
+    <t>NCP699SN33</t>
+  </si>
+  <si>
+    <t>STI3508</t>
+  </si>
+  <si>
+    <t>RANGO VOLTAJE V</t>
+  </si>
+  <si>
+    <t>RIN Ohm</t>
+  </si>
+  <si>
+    <t>ROUT Ohm</t>
+  </si>
+  <si>
+    <t>sensor de agua</t>
+  </si>
+  <si>
+    <t>sensor de corriente DC</t>
+  </si>
+  <si>
+    <t>Amplificador op</t>
+  </si>
+  <si>
+    <t>sensor de temperatura y humedad relativa</t>
+  </si>
+  <si>
+    <t>Sensor de corriente AC y DC</t>
+  </si>
+  <si>
+    <t>Microcontrolador</t>
+  </si>
+  <si>
+    <t>Resistencia indicadora bateria cargada</t>
+  </si>
+  <si>
+    <t>Resistencia indicadora bateria descargada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulo comunicación </t>
+  </si>
+  <si>
+    <t>Regulador de voltaje</t>
+  </si>
+  <si>
+    <t>Convertidor Step-Up</t>
+  </si>
+  <si>
+    <t>2-24</t>
+  </si>
+  <si>
+    <t>1Meg</t>
+  </si>
+  <si>
+    <t>80m</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Regulador de voltaje EN atado a VIN</t>
+  </si>
+  <si>
+    <t>5,05-12</t>
+  </si>
+  <si>
+    <t>BW Hz</t>
+  </si>
+  <si>
+    <t>I TYP mA</t>
+  </si>
+  <si>
+    <t>I MAX mA</t>
+  </si>
+  <si>
+    <t>RUIDO UV</t>
+  </si>
+  <si>
+    <t>1,2K</t>
+  </si>
+  <si>
+    <t>13,8K @1MhZ</t>
+  </si>
+  <si>
+    <t>3,3-6</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>40mA</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>medir corriente agua</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3-5,5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1,8-5,5</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>20M</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>0,007</t>
+  </si>
+  <si>
+    <t>2,560</t>
+  </si>
+  <si>
+    <t>3,5-5,1; 1,8; 1,7-5,5</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>4,5-5,0</t>
+  </si>
+  <si>
+    <t>80k</t>
+  </si>
+  <si>
+    <t>minimo 4,7k</t>
+  </si>
+  <si>
+    <t>2,7-6</t>
+  </si>
+  <si>
+    <t>1 m</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>40m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 </t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>1,75</t>
+  </si>
+  <si>
+    <t>1,8-6</t>
+  </si>
+  <si>
+    <t>0,04</t>
+  </si>
+  <si>
+    <t>0,045</t>
+  </si>
+  <si>
+    <t>3,3-5</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>5,5-7</t>
   </si>
 </sst>
 </file>
@@ -421,7 +773,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,8 +792,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -464,11 +840,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,11 +885,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,11 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A140D29A-C849-43EE-A92C-41874705CDFA}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,30 +1250,41 @@
     <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="6" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="0.44140625" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -856,10 +1301,17 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -875,9 +1327,18 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -893,9 +1354,18 @@
       <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -911,9 +1381,18 @@
       <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -929,9 +1408,18 @@
       <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -947,9 +1435,16 @@
       <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -965,9 +1460,16 @@
       <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -983,9 +1485,16 @@
       <c r="E10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1001,9 +1510,16 @@
       <c r="E11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -1019,9 +1535,16 @@
       <c r="E12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -1037,9 +1560,16 @@
       <c r="E13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1055,9 +1585,16 @@
       <c r="E14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1073,9 +1610,16 @@
       <c r="E15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1091,9 +1635,16 @@
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -1109,9 +1660,16 @@
       <c r="E17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1127,9 +1685,16 @@
       <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1145,9 +1710,16 @@
       <c r="E19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1163,32 +1735,46 @@
       <c r="E20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -1197,11 +1783,18 @@
         <v>24</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1212,19 +1805,26 @@
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="B24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="4">
         <v>20</v>
@@ -1233,16 +1833,23 @@
         <v>24</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="4">
         <v>35</v>
@@ -1251,34 +1858,48 @@
         <v>24</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C26" s="4">
         <v>3</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -1287,16 +1908,23 @@
         <v>24</v>
       </c>
       <c r="E27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="B28" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="4">
         <v>1</v>
@@ -1305,11 +1933,18 @@
         <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
@@ -1320,19 +1955,26 @@
         <v>4</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="4">
         <v>3</v>
@@ -1341,16 +1983,23 @@
         <v>24</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
@@ -1359,250 +2008,348 @@
         <v>24</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="4">
         <v>3</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C33" s="4">
         <v>3</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" s="4">
         <v>5</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C35" s="4">
         <v>1</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="4">
         <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4">
         <v>1</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" s="4">
         <v>1</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="4">
         <v>1</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="4">
+        <v>3</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="4">
-        <v>2</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C43" s="4">
         <v>2</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C45" s="4">
         <v>1</v>
@@ -1611,34 +2358,48 @@
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="C46" s="4">
         <v>1</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C47" s="4">
         <v>1</v>
@@ -1647,16 +2408,23 @@
         <v>24</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C48" s="4">
         <v>2</v>
@@ -1665,16 +2433,23 @@
         <v>180</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C49" s="4">
         <v>1</v>
@@ -1683,74 +2458,1515 @@
         <v>24</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="4">
+        <v>10</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="4">
+        <v>3</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="4">
+        <v>4</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="4">
+        <v>3</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="4">
+        <v>2</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="4">
+        <v>5</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="4">
+        <v>5</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" s="4">
+        <v>2</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="4">
+        <v>5</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="4">
+        <v>4</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="4">
+        <v>4</v>
+      </c>
+      <c r="D60" s="4">
+        <v>91</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="4">
+        <v>5</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="4">
+        <v>5</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="4">
+        <v>10</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="4">
+        <v>5</v>
+      </c>
+      <c r="D64" s="4">
+        <v>10</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="4">
+        <v>5</v>
+      </c>
+      <c r="D65" s="4">
+        <v>5</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="4">
+        <v>3</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="4">
+        <v>4</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="4">
+        <v>2</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="4">
+        <v>2</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="4">
+        <v>2</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="4">
+        <v>3</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="4">
+        <v>2</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" s="4">
+        <v>1</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="4">
+        <v>1</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="7"/>
+      <c r="K84" s="7"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="7"/>
+      <c r="K88" s="7"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="7"/>
+      <c r="K96" s="7"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="7"/>
+      <c r="J98" s="7"/>
+      <c r="K98" s="7"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7"/>
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7"/>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="7"/>
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
+      <c r="G117" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="I118" s="7"/>
+      <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
+      <c r="G119" s="7"/>
+      <c r="H119" s="7"/>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
+      <c r="G120" s="7"/>
+      <c r="H120" s="7"/>
+      <c r="I120" s="7"/>
+      <c r="J120" s="7"/>
+      <c r="K120" s="7"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
+      <c r="G121" s="7"/>
+      <c r="H121" s="7"/>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
+      <c r="G122" s="7"/>
+      <c r="H122" s="7"/>
+      <c r="I122" s="7"/>
+      <c r="J122" s="7"/>
+      <c r="K122" s="7"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
+      <c r="G123" s="7"/>
+      <c r="H123" s="7"/>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
+      <c r="G124" s="7"/>
+      <c r="H124" s="7"/>
+      <c r="I124" s="7"/>
+      <c r="J124" s="7"/>
+      <c r="K124" s="7"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="7"/>
+      <c r="H125" s="7"/>
+      <c r="I125" s="7"/>
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
+      <c r="G126" s="7"/>
+      <c r="H126" s="7"/>
+      <c r="I126" s="7"/>
+      <c r="J126" s="7"/>
+      <c r="K126" s="7"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7"/>
+      <c r="G127" s="7"/>
+      <c r="H127" s="7"/>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
+      <c r="G128" s="7"/>
+      <c r="H128" s="7"/>
+      <c r="I128" s="7"/>
+      <c r="J128" s="7"/>
+      <c r="K128" s="7"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
+      <c r="G129" s="7"/>
+      <c r="H129" s="7"/>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
+      <c r="G130" s="7"/>
+      <c r="H130" s="7"/>
+      <c r="I130" s="7"/>
+      <c r="J130" s="7"/>
+      <c r="K130" s="7"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7"/>
+      <c r="G131" s="7"/>
+      <c r="H131" s="7"/>
+      <c r="I131" s="7"/>
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
+      <c r="G132" s="7"/>
+      <c r="H132" s="7"/>
+      <c r="I132" s="7"/>
+      <c r="J132" s="7"/>
+      <c r="K132" s="7"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="7"/>
+      <c r="H133" s="7"/>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
+      <c r="G134" s="7"/>
+      <c r="H134" s="7"/>
+      <c r="I134" s="7"/>
+      <c r="J134" s="7"/>
+      <c r="K134" s="7"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135" s="7"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7"/>
+      <c r="G135" s="7"/>
+      <c r="H135" s="7"/>
+      <c r="I135" s="7"/>
+      <c r="J135" s="7"/>
+      <c r="K135" s="7"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
+      <c r="G136" s="7"/>
+      <c r="H136" s="7"/>
+      <c r="I136" s="7"/>
+      <c r="J136" s="7"/>
+      <c r="K136" s="7"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137" s="7"/>
+      <c r="B137" s="7"/>
+      <c r="C137" s="7"/>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7"/>
+      <c r="G137" s="7"/>
+      <c r="H137" s="7"/>
+      <c r="I137" s="7"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="C138" s="7"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="7"/>
+      <c r="G138" s="7"/>
+      <c r="H138" s="7"/>
+      <c r="I138" s="7"/>
+      <c r="J138" s="7"/>
+      <c r="K138" s="7"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A139" s="7"/>
+      <c r="B139" s="7"/>
+      <c r="C139" s="7"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7"/>
+      <c r="G139" s="7"/>
+      <c r="H139" s="7"/>
+      <c r="I139" s="7"/>
+      <c r="J139" s="7"/>
+      <c r="K139" s="7"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="7"/>
+      <c r="H140" s="7"/>
+      <c r="I140" s="7"/>
+      <c r="J140" s="7"/>
+      <c r="K140" s="7"/>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+      <c r="C141" s="7"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7"/>
+      <c r="G141" s="7"/>
+      <c r="H141" s="7"/>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A56" xr:uid="{8B46BAFA-F2DE-4EB5-BAD2-8778360EA1A4}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="BORNERA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:B88" xr:uid="{3D27DF11-11B8-4D23-8571-FD77C481583A}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>
   </mergeCells>
@@ -1758,4 +3974,766 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDE412E-7748-42A7-AF32-1116F17F9EFE}">
+  <dimension ref="A1:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="18">
+        <v>10</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I14" s="18">
+        <v>24</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="18">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
avance en esquematico para la PCB
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="585" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{418BC232-AD1E-47F5-B599-B1E242310D00}"/>
+  <xr:revisionPtr revIDLastSave="921" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{087A7680-D3A5-45A2-87BA-F5903D56DEF0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1830" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPONENTES" sheetId="1" r:id="rId1"/>
     <sheet name="CARACTERISTICAS" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPONENTES!$A$3:$B$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CARACTERISTICAS!$C$1:$C$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPONENTES!$A$3:$D$74</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="230">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -469,9 +471,6 @@
     <t>SENSOR DE CORRIENTE SALIDA VOLTAJE</t>
   </si>
   <si>
-    <t>MMCP15501-18 E/SN</t>
-  </si>
-  <si>
     <t>1,8V</t>
   </si>
   <si>
@@ -526,12 +525,6 @@
     <t>MCP33121</t>
   </si>
   <si>
-    <t>R-BATH</t>
-  </si>
-  <si>
-    <t>T-BATL</t>
-  </si>
-  <si>
     <t>XBEE</t>
   </si>
   <si>
@@ -559,9 +552,6 @@
     <t>ROUT Ohm</t>
   </si>
   <si>
-    <t>sensor de agua</t>
-  </si>
-  <si>
     <t>sensor de corriente DC</t>
   </si>
   <si>
@@ -577,12 +567,6 @@
     <t>Microcontrolador</t>
   </si>
   <si>
-    <t>Resistencia indicadora bateria cargada</t>
-  </si>
-  <si>
-    <t>Resistencia indicadora bateria descargada</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modulo comunicación </t>
   </si>
   <si>
@@ -628,18 +612,9 @@
     <t>13,8K @1MhZ</t>
   </si>
   <si>
-    <t>3,3-6</t>
-  </si>
-  <si>
-    <t>1,5</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>40mA</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -649,36 +624,18 @@
     <t>5</t>
   </si>
   <si>
-    <t>3-5,5</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>1,8-5,5</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
     <t>20M</t>
   </si>
   <si>
     <t>90</t>
   </si>
   <si>
-    <t>0,007</t>
-  </si>
-  <si>
-    <t>2,560</t>
-  </si>
-  <si>
-    <t>3,5-5,1; 1,8; 1,7-5,5</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
@@ -691,52 +648,88 @@
     <t>minimo 4,7k</t>
   </si>
   <si>
-    <t>2,7-6</t>
-  </si>
-  <si>
-    <t>1 m</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>40m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 </t>
-  </si>
-  <si>
-    <t>3,3</t>
-  </si>
-  <si>
     <t>0,1</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>1,75</t>
-  </si>
-  <si>
-    <t>1,8-6</t>
-  </si>
-  <si>
-    <t>0,04</t>
-  </si>
-  <si>
-    <t>0,045</t>
-  </si>
-  <si>
-    <t>3,3-5</t>
-  </si>
-  <si>
     <t>55</t>
   </si>
   <si>
     <t>5,5-7</t>
+  </si>
+  <si>
+    <t>sensor de agua alimentar a 5</t>
+  </si>
+  <si>
+    <t>VOLTAJE RECOMENDADO</t>
+  </si>
+  <si>
+    <t>3.3-6</t>
+  </si>
+  <si>
+    <t>3-5.5</t>
+  </si>
+  <si>
+    <t>1.8-5.5</t>
+  </si>
+  <si>
+    <t>3.5-5.1; 1.8; 1.7-5.5</t>
+  </si>
+  <si>
+    <t>2.7-6</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>1.8-6</t>
+  </si>
+  <si>
+    <t>3.3-5</t>
+  </si>
+  <si>
+    <t>1.75</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>5,1.8,(3.3,5)</t>
+  </si>
+  <si>
+    <t>XBEE REG</t>
+  </si>
+  <si>
+    <t>REF3450-MCP18-XBEE</t>
+  </si>
+  <si>
+    <t>195mA</t>
+  </si>
+  <si>
+    <t>LP3869-1</t>
+  </si>
+  <si>
+    <t>LP3869-2</t>
+  </si>
+  <si>
+    <t>PLANIFICADOS PARA PCB</t>
+  </si>
+  <si>
+    <t>CAPACITOR 2,2UF</t>
+  </si>
+  <si>
+    <t>REGISTRAR TEMPERATURA DOCUMENTO</t>
+  </si>
+  <si>
+    <t>MCP1501-18 E/SN</t>
   </si>
 </sst>
 </file>
@@ -870,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -893,18 +886,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -912,16 +929,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1238,10 +1255,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A140D29A-C849-43EE-A92C-41874705CDFA}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,18 +1271,18 @@
     <col min="5" max="5" width="66.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1272,12 +1290,12 @@
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -1311,7 +1329,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1356,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1359,7 +1377,7 @@
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1386,7 +1404,7 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1413,13 +1431,13 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1457,9 @@
         <v>117</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>227</v>
+      </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1464,12 +1484,14 @@
         <v>117</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>228</v>
+      </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1494,7 +1516,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1541,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -1544,7 +1566,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -1569,7 +1591,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1594,7 +1616,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1619,7 +1641,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1644,7 +1666,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -1669,7 +1691,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +1716,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1719,7 +1741,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1744,7 +1766,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -1769,7 +1791,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
@@ -1794,7 +1816,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1819,7 +1841,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
@@ -1844,7 +1866,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>52</v>
       </c>
@@ -1869,7 +1891,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -1894,7 +1916,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
@@ -1919,7 +1941,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>65</v>
       </c>
@@ -1969,7 +1991,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -1994,7 +2016,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>69</v>
       </c>
@@ -2019,7 +2041,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -2044,7 +2066,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -2069,7 +2091,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2116,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -2144,7 +2166,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -2169,7 +2191,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>69</v>
       </c>
@@ -2194,7 +2216,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
@@ -2219,7 +2241,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -2244,7 +2266,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
@@ -2269,7 +2291,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -2294,7 +2316,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
@@ -2319,7 +2341,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -2344,7 +2366,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
@@ -2369,7 +2391,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>104</v>
       </c>
@@ -2394,7 +2416,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -2419,7 +2441,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>109</v>
       </c>
@@ -2444,7 +2466,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2694,7 +2716,7 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>7</v>
       </c>
@@ -2719,7 +2741,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>7</v>
       </c>
@@ -2744,7 +2766,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2769,7 +2791,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2794,7 +2816,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2819,7 +2841,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2844,7 +2866,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -2869,7 +2891,7 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -2894,7 +2916,7 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>21</v>
       </c>
@@ -2919,7 +2941,7 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>31</v>
       </c>
@@ -2944,21 +2966,21 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="C69" s="4">
         <v>2</v>
       </c>
       <c r="D69" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>120</v>
@@ -2969,21 +2991,21 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C70" s="4">
         <v>2</v>
       </c>
       <c r="D70" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>120</v>
@@ -2994,12 +3016,12 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="C71" s="4">
         <v>3</v>
@@ -3008,7 +3030,7 @@
         <v>71</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>117</v>
@@ -3019,12 +3041,12 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C72" s="4">
         <v>2</v>
@@ -3033,7 +3055,7 @@
         <v>26</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>117</v>
@@ -3044,12 +3066,12 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C73" s="4">
         <v>1</v>
@@ -3069,12 +3091,12 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C74" s="4">
         <v>1</v>
@@ -3083,7 +3105,7 @@
         <v>71</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>117</v>
@@ -3966,7 +3988,13 @@
       <c r="K141" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B88" xr:uid="{3D27DF11-11B8-4D23-8571-FD77C481583A}"/>
+  <autoFilter ref="A3:D74" xr:uid="{6DF3D42B-872E-4793-906A-E79819EBEDA4}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CAPACITOR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>
   </mergeCells>
@@ -3978,745 +4006,745 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDE412E-7748-42A7-AF32-1116F17F9EFE}">
-  <dimension ref="A1:M35"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5546875" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="23"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="17">
+        <v>40</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="17">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="B5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="F5" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="C6" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="18">
+        <v>65</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="K6" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>161</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="17">
+        <v>16</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="D10" s="18">
+        <v>40</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="18">
+        <v>23</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="12">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I12" s="12">
+        <v>24</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="D13" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C15" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="G15" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="H15" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="18">
-        <v>10</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I14" s="18">
-        <v>24</v>
-      </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="D17" s="18">
-        <v>2</v>
-      </c>
-      <c r="E17" s="18">
-        <v>1.6</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C15" xr:uid="{28BC0D4C-5BAD-43AD-B979-D66A489712BD}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1,8-5,5"/>
+        <filter val="1,8-6"/>
+        <filter val="2,7-6"/>
+        <filter val="2-24"/>
+        <filter val="3,3"/>
+        <filter val="3,3-5"/>
+        <filter val="3,3-6"/>
+        <filter val="3,5-5,1; 1,8; 1,7-5,5"/>
+        <filter val="3-5,5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="13">
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
@@ -4736,4 +4764,176 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F71BFCC-ECE2-4A3A-9AC7-F0EE5D0BF03B}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
terminacion de esquematico e inicio del esquematico del coordinador
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="921" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{087A7680-D3A5-45A2-87BA-F5903D56DEF0}"/>
+  <xr:revisionPtr revIDLastSave="935" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E91FB4DB-0F97-4558-B147-CA5B785683C4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="232">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -730,6 +730,12 @@
   </si>
   <si>
     <t>MCP1501-18 E/SN</t>
+  </si>
+  <si>
+    <t>0,8</t>
+  </si>
+  <si>
+    <t>LAS MEDIDAS DE la INA NO PUEDEN SER SIN SIGNO</t>
   </si>
 </sst>
 </file>
@@ -863,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -911,6 +917,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -931,9 +943,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1255,11 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A140D29A-C849-43EE-A92C-41874705CDFA}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1271,18 +1279,18 @@
     <col min="5" max="5" width="66.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0.44140625" customWidth="1"/>
-    <col min="8" max="8" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1290,12 +1298,12 @@
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -1329,7 +1337,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1356,7 +1364,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1445,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1491,7 +1499,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1511,12 +1519,14 @@
         <v>117</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="20" t="s">
+        <v>231</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1541,7 +1551,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -1566,7 +1576,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -1591,7 +1601,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1616,7 +1626,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1641,7 +1651,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +1676,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -1691,7 +1701,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1716,7 +1726,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1741,7 +1751,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1766,7 +1776,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -1791,7 +1801,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
@@ -1816,7 +1826,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1841,7 +1851,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +1876,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>52</v>
       </c>
@@ -1891,7 +1901,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -1916,7 +1926,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
@@ -1941,7 +1951,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>65</v>
       </c>
@@ -1986,12 +1996,11 @@
         <v>117</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2016,7 +2025,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>69</v>
       </c>
@@ -2041,7 +2050,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -2066,7 +2075,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -2091,7 +2100,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -2116,7 +2125,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -2166,7 +2175,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -2191,7 +2200,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>69</v>
       </c>
@@ -2216,7 +2225,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
@@ -2241,7 +2250,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -2266,7 +2275,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
@@ -2291,7 +2300,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -2316,7 +2325,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
@@ -2341,7 +2350,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -2366,7 +2375,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
@@ -2391,7 +2400,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>104</v>
       </c>
@@ -2416,7 +2425,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -2441,7 +2450,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>109</v>
       </c>
@@ -2466,7 +2475,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2716,7 +2725,7 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>7</v>
       </c>
@@ -2741,7 +2750,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>7</v>
       </c>
@@ -2766,7 +2775,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2791,7 +2800,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2816,7 +2825,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2841,7 +2850,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2866,7 +2875,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -2891,7 +2900,7 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -2916,7 +2925,7 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>21</v>
       </c>
@@ -2941,7 +2950,7 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>31</v>
       </c>
@@ -2966,7 +2975,7 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>58</v>
       </c>
@@ -2991,7 +3000,7 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
@@ -3016,7 +3025,7 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>149</v>
       </c>
@@ -3041,7 +3050,7 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>149</v>
       </c>
@@ -3066,7 +3075,7 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>21</v>
       </c>
@@ -3091,7 +3100,7 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>21</v>
       </c>
@@ -3988,13 +3997,7 @@
       <c r="K141" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:D74" xr:uid="{6DF3D42B-872E-4793-906A-E79819EBEDA4}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="CAPACITOR"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:D74" xr:uid="{6DF3D42B-872E-4793-906A-E79819EBEDA4}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>
   </mergeCells>
@@ -4010,7 +4013,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4029,54 +4032,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -4124,10 +4127,10 @@
         <v>208</v>
       </c>
       <c r="D4" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>181</v>
@@ -4781,152 +4784,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
avances en placing de la pcb del transmisor
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="935" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E91FB4DB-0F97-4558-B147-CA5B785683C4}"/>
+  <xr:revisionPtr revIDLastSave="940" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B17B8A78-7A44-470C-986F-02BCBC1AE95F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="233">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -736,6 +736,9 @@
   </si>
   <si>
     <t>LAS MEDIDAS DE la INA NO PUEDEN SER SIN SIGNO</t>
+  </si>
+  <si>
+    <t>capacitor 10uF ceramico CL31A106KOHNNNE para el regulador de la XBEE</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -891,7 +894,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -926,12 +928,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -939,6 +935,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,6 +951,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1267,7 +1278,7 @@
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,14 +1294,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1298,12 +1309,12 @@
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -1357,7 +1368,7 @@
         <v>117</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="29" t="s">
         <v>130</v>
       </c>
       <c r="I4" s="7"/>
@@ -1384,7 +1395,7 @@
         <v>117</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="29" t="s">
         <v>154</v>
       </c>
       <c r="I5" s="7"/>
@@ -1411,7 +1422,7 @@
         <v>117</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="29" t="s">
         <v>157</v>
       </c>
       <c r="I6" s="7"/>
@@ -1438,7 +1449,7 @@
         <v>117</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="30" t="s">
         <v>192</v>
       </c>
       <c r="I7" s="7"/>
@@ -1465,7 +1476,7 @@
         <v>117</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="30" t="s">
         <v>227</v>
       </c>
       <c r="I8" s="7"/>
@@ -1492,7 +1503,7 @@
         <v>117</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="30" t="s">
         <v>228</v>
       </c>
       <c r="I9" s="7"/>
@@ -1519,14 +1530,14 @@
         <v>117</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="19" t="s">
         <v>231</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1546,7 +1557,9 @@
         <v>117</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="30" t="s">
+        <v>232</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -1571,7 +1584,7 @@
         <v>117</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -1596,7 +1609,7 @@
         <v>117</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -1621,7 +1634,7 @@
         <v>117</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -1646,7 +1659,7 @@
         <v>117</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -1671,7 +1684,7 @@
         <v>117</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
@@ -1696,7 +1709,7 @@
         <v>117</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -1721,7 +1734,7 @@
         <v>117</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="31"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -1746,7 +1759,7 @@
         <v>117</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -1771,7 +1784,7 @@
         <v>117</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -4032,659 +4045,659 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>40</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>159</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>1.5</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>139</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>65</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>160</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>2.5</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>141</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12" t="s">
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>16</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12" t="s">
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>161</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>40</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12" t="s">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>162</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>23</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12" t="s">
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>163</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <v>24</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>164</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>165</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12" t="s">
+      <c r="I14" s="11"/>
+      <c r="J14" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>166</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>2</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
@@ -4695,9 +4708,9 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -4708,9 +4721,9 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
@@ -4749,6 +4762,11 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="F1:F2"/>
@@ -4757,11 +4775,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4784,152 +4797,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
screen ino verified screen and placing in receiving corrected
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="950" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E5B25CA-E6E3-4E9E-BA3C-F20E58AE8088}"/>
+  <xr:revisionPtr revIDLastSave="953" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7FB99BF2-B12C-46C1-955B-1370FD2F5063}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="240">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -754,6 +754,12 @@
   </si>
   <si>
     <t>BOTON</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>Alcohol Isoprop</t>
   </si>
 </sst>
 </file>
@@ -1292,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A140D29A-C849-43EE-A92C-41874705CDFA}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,7 +1740,9 @@
         <v>117</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="22"/>
+      <c r="H17" s="19" t="s">
+        <v>238</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -1759,7 +1767,9 @@
         <v>117</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="22" t="s">
+        <v>239</v>
+      </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>

</xml_diff>

<commit_message>
pcb enviadas a produccion
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="953" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7FB99BF2-B12C-46C1-955B-1370FD2F5063}"/>
+  <xr:revisionPtr revIDLastSave="966" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6DA58E16-51B7-4A47-A402-FBAF5132EF42}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="242">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -760,6 +760,12 @@
   </si>
   <si>
     <t>Alcohol Isoprop</t>
+  </si>
+  <si>
+    <t>Cinta para desoldar</t>
+  </si>
+  <si>
+    <t>Pines</t>
   </si>
 </sst>
 </file>
@@ -893,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -952,9 +958,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,6 +984,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1296,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A140D29A-C849-43EE-A92C-41874705CDFA}">
-  <dimension ref="A1:K141"/>
+  <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,35 +1323,39 @@
     <col min="8" max="8" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1368,8 +1381,10 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1395,8 +1410,10 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1416,14 +1433,16 @@
         <v>117</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="32" t="s">
         <v>233</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1443,14 +1462,16 @@
         <v>117</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="32" t="s">
         <v>156</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1476,8 +1497,10 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1503,8 +1526,10 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1530,8 +1555,10 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1557,8 +1584,10 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1578,14 +1607,16 @@
         <v>117</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="32" t="s">
         <v>231</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -1605,14 +1636,16 @@
         <v>117</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="32" t="s">
         <v>232</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -1632,14 +1665,16 @@
         <v>117</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="31" t="s">
         <v>234</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1659,14 +1694,16 @@
         <v>117</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="31" t="s">
         <v>235</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1686,14 +1723,16 @@
         <v>117</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="31" t="s">
         <v>236</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1713,14 +1752,16 @@
         <v>117</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="31" t="s">
         <v>237</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -1740,14 +1781,16 @@
         <v>117</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="31" t="s">
         <v>238</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1767,14 +1810,16 @@
         <v>117</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="31" t="s">
         <v>239</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1794,12 +1839,16 @@
         <v>117</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="22"/>
+      <c r="H19" s="31" t="s">
+        <v>240</v>
+      </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1819,12 +1868,16 @@
         <v>117</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="22"/>
+      <c r="H20" s="31" t="s">
+        <v>241</v>
+      </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -1848,8 +1901,10 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
@@ -1873,8 +1928,10 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1898,8 +1955,10 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
@@ -1923,8 +1982,10 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>52</v>
       </c>
@@ -1948,8 +2009,10 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -1973,8 +2036,10 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
@@ -1998,8 +2063,10 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>65</v>
       </c>
@@ -2023,8 +2090,10 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
@@ -2047,8 +2116,10 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2072,8 +2143,10 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>69</v>
       </c>
@@ -2097,8 +2170,10 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -2122,8 +2197,10 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -2147,8 +2224,10 @@
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -2172,8 +2251,10 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -2197,8 +2278,10 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
@@ -2222,8 +2305,10 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -2247,8 +2332,10 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>69</v>
       </c>
@@ -2272,8 +2359,10 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
@@ -2297,8 +2386,10 @@
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -2322,8 +2413,10 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
@@ -2347,8 +2440,10 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -2372,8 +2467,10 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
@@ -2397,8 +2494,10 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -2422,8 +2521,10 @@
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
@@ -2447,8 +2548,10 @@
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>104</v>
       </c>
@@ -2472,8 +2575,10 @@
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -2497,8 +2602,10 @@
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>109</v>
       </c>
@@ -2522,8 +2629,10 @@
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2547,8 +2656,10 @@
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>8</v>
       </c>
@@ -2572,8 +2683,10 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
@@ -2597,8 +2710,10 @@
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>8</v>
       </c>
@@ -2622,8 +2737,10 @@
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
@@ -2647,8 +2764,10 @@
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
@@ -2672,8 +2791,10 @@
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>8</v>
       </c>
@@ -2697,8 +2818,10 @@
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>8</v>
       </c>
@@ -2722,8 +2845,10 @@
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>8</v>
       </c>
@@ -2747,8 +2872,10 @@
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>8</v>
       </c>
@@ -2772,8 +2899,10 @@
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>7</v>
       </c>
@@ -2797,8 +2926,10 @@
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>7</v>
       </c>
@@ -2822,8 +2953,10 @@
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2847,8 +2980,10 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2872,8 +3007,10 @@
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2897,8 +3034,10 @@
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2922,8 +3061,10 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -2947,8 +3088,10 @@
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -2972,8 +3115,10 @@
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>21</v>
       </c>
@@ -2997,8 +3142,10 @@
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>31</v>
       </c>
@@ -3022,8 +3169,10 @@
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>58</v>
       </c>
@@ -3047,8 +3196,10 @@
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
@@ -3072,8 +3223,10 @@
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>149</v>
       </c>
@@ -3097,8 +3250,10 @@
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>149</v>
       </c>
@@ -3122,8 +3277,10 @@
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>21</v>
       </c>
@@ -3147,8 +3304,10 @@
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>21</v>
       </c>
@@ -3172,8 +3331,10 @@
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3185,8 +3346,10 @@
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3198,8 +3361,10 @@
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3211,8 +3376,10 @@
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3224,8 +3391,10 @@
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3237,8 +3406,10 @@
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79" s="7"/>
+      <c r="M79" s="7"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3250,8 +3421,10 @@
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80" s="7"/>
+      <c r="M80" s="7"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3263,8 +3436,10 @@
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3276,8 +3451,10 @@
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82" s="7"/>
+      <c r="M82" s="7"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3289,8 +3466,10 @@
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3302,8 +3481,10 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84" s="7"/>
+      <c r="M84" s="7"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3315,8 +3496,10 @@
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3328,8 +3511,10 @@
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L86" s="7"/>
+      <c r="M86" s="7"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3341,8 +3526,10 @@
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L87" s="7"/>
+      <c r="M87" s="7"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3354,8 +3541,10 @@
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L88" s="7"/>
+      <c r="M88" s="7"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="4"/>
@@ -3367,8 +3556,10 @@
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L89" s="7"/>
+      <c r="M89" s="7"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="4"/>
@@ -3380,8 +3571,10 @@
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L90" s="7"/>
+      <c r="M90" s="7"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="4"/>
@@ -3393,8 +3586,10 @@
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L91" s="7"/>
+      <c r="M91" s="7"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4"/>
@@ -3406,8 +3601,10 @@
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L92" s="7"/>
+      <c r="M92" s="7"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="4"/>
@@ -3419,8 +3616,10 @@
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L93" s="7"/>
+      <c r="M93" s="7"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="4"/>
@@ -3432,8 +3631,10 @@
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="4"/>
@@ -3445,8 +3646,10 @@
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L95" s="7"/>
+      <c r="M95" s="7"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="4"/>
@@ -3458,8 +3661,10 @@
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L96" s="7"/>
+      <c r="M96" s="7"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="4"/>
@@ -3471,8 +3676,10 @@
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L97" s="7"/>
+      <c r="M97" s="7"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="4"/>
@@ -3484,8 +3691,10 @@
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L98" s="7"/>
+      <c r="M98" s="7"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="4"/>
@@ -3497,8 +3706,10 @@
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L99" s="7"/>
+      <c r="M99" s="7"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="4"/>
@@ -3510,8 +3721,10 @@
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L100" s="7"/>
+      <c r="M100" s="7"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="4"/>
@@ -3523,8 +3736,10 @@
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L101" s="7"/>
+      <c r="M101" s="7"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="4"/>
@@ -3536,8 +3751,10 @@
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L102" s="7"/>
+      <c r="M102" s="7"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="4"/>
@@ -3549,8 +3766,10 @@
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L103" s="7"/>
+      <c r="M103" s="7"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="4"/>
@@ -3562,8 +3781,10 @@
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L104" s="7"/>
+      <c r="M104" s="7"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3575,8 +3796,10 @@
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L105" s="7"/>
+      <c r="M105" s="7"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3588,8 +3811,10 @@
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L106" s="7"/>
+      <c r="M106" s="7"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3601,8 +3826,10 @@
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L107" s="7"/>
+      <c r="M107" s="7"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3614,8 +3841,10 @@
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L108" s="7"/>
+      <c r="M108" s="7"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -3627,8 +3856,10 @@
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L109" s="7"/>
+      <c r="M109" s="7"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -3640,8 +3871,10 @@
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L110" s="7"/>
+      <c r="M110" s="7"/>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -3653,8 +3886,10 @@
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L111" s="7"/>
+      <c r="M111" s="7"/>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -3666,8 +3901,10 @@
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L112" s="7"/>
+      <c r="M112" s="7"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -3679,8 +3916,10 @@
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L113" s="7"/>
+      <c r="M113" s="7"/>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -3692,8 +3931,10 @@
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L114" s="7"/>
+      <c r="M114" s="7"/>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -3705,8 +3946,10 @@
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L115" s="7"/>
+      <c r="M115" s="7"/>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -3718,8 +3961,10 @@
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L116" s="7"/>
+      <c r="M116" s="7"/>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -3731,8 +3976,10 @@
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L117" s="7"/>
+      <c r="M117" s="7"/>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -3744,8 +3991,10 @@
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L118" s="7"/>
+      <c r="M118" s="7"/>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -3757,8 +4006,10 @@
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L119" s="7"/>
+      <c r="M119" s="7"/>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -3770,8 +4021,10 @@
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L120" s="7"/>
+      <c r="M120" s="7"/>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -3783,8 +4036,10 @@
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L121" s="7"/>
+      <c r="M121" s="7"/>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -3796,8 +4051,10 @@
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L122" s="7"/>
+      <c r="M122" s="7"/>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -3809,8 +4066,10 @@
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L123" s="7"/>
+      <c r="M123" s="7"/>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -3822,8 +4081,10 @@
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L124" s="7"/>
+      <c r="M124" s="7"/>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
@@ -3835,8 +4096,10 @@
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L125" s="7"/>
+      <c r="M125" s="7"/>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
@@ -3848,8 +4111,10 @@
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L126" s="7"/>
+      <c r="M126" s="7"/>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
@@ -3861,8 +4126,10 @@
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L127" s="7"/>
+      <c r="M127" s="7"/>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -3874,8 +4141,10 @@
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L128" s="7"/>
+      <c r="M128" s="7"/>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -3887,8 +4156,10 @@
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L129" s="7"/>
+      <c r="M129" s="7"/>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -3900,8 +4171,10 @@
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L130" s="7"/>
+      <c r="M130" s="7"/>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -3913,8 +4186,10 @@
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L131" s="7"/>
+      <c r="M131" s="7"/>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
@@ -3926,8 +4201,10 @@
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L132" s="7"/>
+      <c r="M132" s="7"/>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
@@ -3939,8 +4216,10 @@
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L133" s="7"/>
+      <c r="M133" s="7"/>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -3952,8 +4231,10 @@
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L134" s="7"/>
+      <c r="M134" s="7"/>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -3965,8 +4246,10 @@
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L135" s="7"/>
+      <c r="M135" s="7"/>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -3978,8 +4261,10 @@
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L136" s="7"/>
+      <c r="M136" s="7"/>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -3992,7 +4277,7 @@
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -4005,7 +4290,7 @@
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -4018,7 +4303,7 @@
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -4031,7 +4316,7 @@
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -4080,54 +4365,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -4832,22 +5117,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>

</xml_diff>

<commit_message>
edicion de codigo para energia solamente... pruebas
</commit_message>
<xml_diff>
--- a/PCB/INVENTARIO.xlsx
+++ b/PCB/INVENTARIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a3ac2fae305033/Escritorio/ModComT/ModuloComunicacion/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="966" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6DA58E16-51B7-4A47-A402-FBAF5132EF42}"/>
+  <xr:revisionPtr revIDLastSave="978" documentId="6_{E4BA928A-FD9E-47B9-8872-964245846C8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B0DA93A6-725E-4830-B3CA-A7E2B91DE58E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
+    <workbookView minimized="1" xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{D4F0B476-1E35-42B6-8334-B0BB6DF98FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPONENTES" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="244">
   <si>
     <t>INVENTARIO</t>
   </si>
@@ -766,6 +766,12 @@
   </si>
   <si>
     <t>Pines</t>
+  </si>
+  <si>
+    <t>cama atmega</t>
+  </si>
+  <si>
+    <t>C 100nf</t>
   </si>
 </sst>
 </file>
@@ -958,13 +964,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -976,6 +982,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -984,12 +996,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A140D29A-C849-43EE-A92C-41874705CDFA}">
   <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,14 +1330,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1341,12 +1347,12 @@
       <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -1433,7 +1439,7 @@
         <v>117</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="23" t="s">
         <v>233</v>
       </c>
       <c r="I5" s="7"/>
@@ -1462,7 +1468,7 @@
         <v>117</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="23" t="s">
         <v>156</v>
       </c>
       <c r="I6" s="7"/>
@@ -1607,7 +1613,7 @@
         <v>117</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="23" t="s">
         <v>231</v>
       </c>
       <c r="I11" s="7"/>
@@ -1636,7 +1642,7 @@
         <v>117</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="23" t="s">
         <v>232</v>
       </c>
       <c r="I12" s="7"/>
@@ -1665,7 +1671,7 @@
         <v>117</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="22" t="s">
         <v>234</v>
       </c>
       <c r="I13" s="7"/>
@@ -1694,7 +1700,7 @@
         <v>117</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="22" t="s">
         <v>235</v>
       </c>
       <c r="I14" s="7"/>
@@ -1723,7 +1729,7 @@
         <v>117</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="22" t="s">
         <v>236</v>
       </c>
       <c r="I15" s="7"/>
@@ -1752,7 +1758,7 @@
         <v>117</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="22" t="s">
         <v>237</v>
       </c>
       <c r="I16" s="7"/>
@@ -1781,7 +1787,7 @@
         <v>117</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="22" t="s">
         <v>238</v>
       </c>
       <c r="I17" s="7"/>
@@ -1810,7 +1816,7 @@
         <v>117</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="22" t="s">
         <v>239</v>
       </c>
       <c r="I18" s="7"/>
@@ -1839,7 +1845,7 @@
         <v>117</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="22" t="s">
         <v>240</v>
       </c>
       <c r="I19" s="7"/>
@@ -1868,7 +1874,7 @@
         <v>117</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="22" t="s">
         <v>241</v>
       </c>
       <c r="I20" s="7"/>
@@ -1897,7 +1903,9 @@
         <v>117</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -1924,7 +1932,9 @@
         <v>117</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="H22" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -4365,19 +4375,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="28" t="s">
         <v>184</v>
       </c>
       <c r="F1" s="26" t="s">
@@ -4386,13 +4396,13 @@
       <c r="G1" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="28" t="s">
         <v>168</v>
       </c>
       <c r="I1" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="28" t="s">
         <v>205</v>
       </c>
       <c r="K1" s="26"/>
@@ -4400,16 +4410,16 @@
       <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="27"/>
       <c r="G2" s="27"/>
-      <c r="H2" s="23"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="27"/>
-      <c r="J2" s="23"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="27"/>
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
@@ -5082,6 +5092,11 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="F1:F2"/>
@@ -5090,11 +5105,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5117,22 +5127,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>

</xml_diff>